<commit_message>
New graphs- total dry biomass by percent col
</commit_message>
<xml_diff>
--- a/Harvest Data.xlsx
+++ b/Harvest Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/demoriegalarza/Desktop/Work/Doug-fir Drought/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/demoriegalarza/Desktop/DFD+DAG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074F2080-0023-594E-9314-53A7BDAE0634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2362D75-4550-704A-99B5-DD52620A11C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4400" yWindow="500" windowWidth="21200" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="206">
   <si>
     <t>NM31</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>DFD_007</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>NM29</t>
@@ -741,7 +738,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -794,7 +791,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1018,8 +1014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819B6F9D-1188-934E-9CF0-4A8F8C7DD01E}">
   <dimension ref="A1:Z90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="S45" sqref="S45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1035,55 +1031,55 @@
   <sheetData>
     <row r="1" spans="1:24" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>185</v>
-      </c>
       <c r="J1" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>193</v>
-      </c>
       <c r="P1" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.15">
@@ -1094,10 +1090,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E2" s="1">
         <v>60.6</v>
@@ -1115,7 +1111,7 @@
         <v>1.3979999999999999</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K2" s="1">
         <v>4.29</v>
@@ -1155,10 +1151,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E3" s="1">
         <v>70</v>
@@ -1176,7 +1172,7 @@
         <v>2.0470000000000002</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K3" s="1">
         <v>3.8035199999999998</v>
@@ -1210,10 +1206,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E4" s="2">
         <v>74.099999999999994</v>
@@ -1231,7 +1227,7 @@
         <v>1.133</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K4" s="2">
         <v>1.958</v>
@@ -1265,10 +1261,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E5" s="2">
         <v>81.599999999999994</v>
@@ -1286,7 +1282,7 @@
         <v>1.212</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K5" s="2">
         <v>2.0289999999999999</v>
@@ -1320,10 +1316,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E6" s="1">
         <v>61.2</v>
@@ -1341,7 +1337,7 @@
         <v>2.2440000000000002</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K6" s="1">
         <v>3.82185</v>
@@ -1375,10 +1371,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E7" s="2">
         <v>65.8</v>
@@ -1396,7 +1392,7 @@
         <v>1.611</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K7" s="2">
         <v>2.0356000000000001</v>
@@ -1430,10 +1426,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E8" s="1">
         <v>70.099999999999994</v>
@@ -1451,7 +1447,7 @@
         <v>1.4984</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K8" s="1">
         <v>3.448</v>
@@ -1479,16 +1475,16 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E9" s="1">
         <v>50.1</v>
@@ -1506,7 +1502,7 @@
         <v>3.0030000000000001</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K9" s="1">
         <v>3.4780000000000002</v>
@@ -1541,16 +1537,16 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E10" s="1">
         <v>52.5</v>
@@ -1568,7 +1564,7 @@
         <v>1.2791600000000001</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K10" s="1">
         <v>0.78600000000000003</v>
@@ -1596,16 +1592,16 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E11" s="2">
         <v>48.3</v>
@@ -1623,7 +1619,7 @@
         <v>2.1102400000000001</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K11" s="2">
         <v>6.1619999999999999</v>
@@ -1651,16 +1647,16 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E12" s="4">
         <v>50</v>
@@ -1678,7 +1674,7 @@
         <v>2.0700099999999999</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K12" s="4">
         <v>3.72</v>
@@ -1706,16 +1702,16 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E13" s="1">
         <v>51.7</v>
@@ -1733,7 +1729,7 @@
         <v>1.9006000000000001</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K13" s="1">
         <v>2.0390000000000001</v>
@@ -1761,16 +1757,16 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E14" s="2">
         <v>48.7</v>
@@ -1788,7 +1784,7 @@
         <v>2.7336999999999998</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K14" s="2">
         <v>3.875</v>
@@ -1816,16 +1812,16 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E15" s="2">
         <v>48.6</v>
@@ -1843,7 +1839,7 @@
         <v>1.88849</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K15" s="2">
         <v>3.6259999999999999</v>
@@ -1871,16 +1867,16 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E16" s="1">
         <v>69.900000000000006</v>
@@ -1898,7 +1894,7 @@
         <v>2.5703</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K16" s="1">
         <v>1.8180000000000001</v>
@@ -1933,16 +1929,16 @@
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E17" s="1">
         <v>69.400000000000006</v>
@@ -1960,7 +1956,7 @@
         <v>2.2650000000000001</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K17" s="1">
         <v>3.0270000000000001</v>
@@ -1988,16 +1984,16 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E18" s="2">
         <v>80.5</v>
@@ -2015,7 +2011,7 @@
         <v>1.2509999999999999</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K18" s="2">
         <v>3.0179999999999998</v>
@@ -2043,16 +2039,16 @@
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E19" s="4">
         <v>67.7</v>
@@ -2070,7 +2066,7 @@
         <v>1.7380899999999999</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K19" s="4">
         <v>0.52300000000000002</v>
@@ -2096,16 +2092,16 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E20" s="2">
         <v>61</v>
@@ -2123,7 +2119,7 @@
         <v>3.0325600000000001</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K20" s="2">
         <v>4.766</v>
@@ -2149,16 +2145,16 @@
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E21" s="1">
         <v>67.3</v>
@@ -2176,7 +2172,7 @@
         <v>3.3971</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K21" s="1">
         <v>4.49</v>
@@ -2204,16 +2200,16 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E22" s="1">
         <v>71.8</v>
@@ -2224,14 +2220,12 @@
       <c r="G22" s="1">
         <v>3.0979999999999999</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="H22" s="1"/>
       <c r="I22" s="1">
         <v>2.5780099999999999</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K22" s="1">
         <v>2.238</v>
@@ -2259,16 +2253,16 @@
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E23" s="1">
         <v>49.5</v>
@@ -2286,7 +2280,7 @@
         <v>2.7604000000000002</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K23" s="1">
         <v>3.4950000000000001</v>
@@ -2321,16 +2315,16 @@
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E24" s="1">
         <v>44.9</v>
@@ -2348,7 +2342,7 @@
         <v>2.206</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K24" s="1">
         <v>4.1120000000000001</v>
@@ -2376,16 +2370,16 @@
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E25" s="1">
         <v>46.7</v>
@@ -2403,7 +2397,7 @@
         <v>2.14</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K25" s="1">
         <v>3.1970000000000001</v>
@@ -2431,16 +2425,16 @@
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E26" s="1">
         <v>73.099999999999994</v>
@@ -2458,7 +2452,7 @@
         <v>1.4770000000000001</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K26" s="1">
         <v>1.4357</v>
@@ -2486,16 +2480,16 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E27" s="2">
         <v>47.5</v>
@@ -2513,7 +2507,7 @@
         <v>2.8519999999999999</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K27" s="2">
         <v>3.6659999999999999</v>
@@ -2541,16 +2535,16 @@
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E28" s="2">
         <v>49.3</v>
@@ -2568,7 +2562,7 @@
         <v>1.3718600000000001</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K28" s="2">
         <v>2.8759999999999999</v>
@@ -2596,16 +2590,16 @@
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E29" s="2">
         <v>51.2</v>
@@ -2623,7 +2617,7 @@
         <v>2.6284999999999998</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K29" s="2">
         <v>4.93</v>
@@ -2651,16 +2645,16 @@
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A30" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E30" s="5">
         <v>67.599999999999994</v>
@@ -2678,7 +2672,7 @@
         <v>3.1321300000000001</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K30" s="5">
         <v>2.5648</v>
@@ -2713,16 +2707,16 @@
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A31" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E31" s="6">
         <v>64.599999999999994</v>
@@ -2740,7 +2734,7 @@
         <v>1.7172000000000001</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K31" s="10">
         <v>5.2245999999999997</v>
@@ -2768,16 +2762,16 @@
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A32" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E32" s="7">
         <v>67.400000000000006</v>
@@ -2795,7 +2789,7 @@
         <v>2.8140000000000001</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K32" s="7">
         <v>7.1459999999999999</v>
@@ -2823,16 +2817,16 @@
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A33" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E33" s="6">
         <v>69</v>
@@ -2850,7 +2844,7 @@
         <v>1.9293</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K33" s="10">
         <v>4.0349000000000004</v>
@@ -2878,16 +2872,16 @@
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A34" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E34" s="5">
         <v>69</v>
@@ -2905,7 +2899,7 @@
         <v>1.583</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K34" s="5">
         <v>5.3268000000000004</v>
@@ -2933,16 +2927,16 @@
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A35" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E35" s="5">
         <v>64.2</v>
@@ -2960,7 +2954,7 @@
         <v>2.2183099999999998</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K35" s="5">
         <v>2.3675000000000002</v>
@@ -2988,16 +2982,16 @@
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A36" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E36" s="7">
         <v>71.2</v>
@@ -3015,7 +3009,7 @@
         <v>1.26955</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K36" s="7">
         <v>2.819</v>
@@ -3043,16 +3037,16 @@
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A37" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E37" s="11">
         <v>46.5</v>
@@ -3070,7 +3064,7 @@
         <v>2.2846299999999999</v>
       </c>
       <c r="J37" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K37" s="11">
         <v>8.01</v>
@@ -3103,16 +3097,16 @@
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A38" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E38" s="12">
         <v>46.7</v>
@@ -3130,7 +3124,7 @@
         <v>1.5205299999999999</v>
       </c>
       <c r="J38" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K38" s="14">
         <v>5.5625999999999998</v>
@@ -3158,16 +3152,16 @@
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A39" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E39" s="12">
         <v>46</v>
@@ -3185,7 +3179,7 @@
         <v>1.7919</v>
       </c>
       <c r="J39" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K39" s="12">
         <v>2.9994999999999998</v>
@@ -3213,16 +3207,16 @@
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A40" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E40" s="11">
         <v>129.6</v>
@@ -3240,7 +3234,7 @@
         <v>1.38964</v>
       </c>
       <c r="J40" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K40" s="13">
         <v>0.41494999999999999</v>
@@ -3268,19 +3262,19 @@
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A41" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F41" s="12">
         <v>1.9</v>
@@ -3295,7 +3289,7 @@
         <v>1.1151</v>
       </c>
       <c r="J41" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K41" s="12">
         <v>2.2669999999999999</v>
@@ -3323,16 +3317,16 @@
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A42" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E42" s="11">
         <v>48.4</v>
@@ -3350,7 +3344,7 @@
         <v>2.4632999999999998</v>
       </c>
       <c r="J42" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K42" s="11">
         <v>4.4850000000000003</v>
@@ -3378,16 +3372,16 @@
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A43" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E43" s="11">
         <v>56.6</v>
@@ -3405,7 +3399,7 @@
         <v>2.3729800000000001</v>
       </c>
       <c r="J43" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K43" s="11">
         <v>2.14</v>
@@ -3433,16 +3427,16 @@
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A44" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E44" s="11">
         <v>67.5</v>
@@ -3460,7 +3454,7 @@
         <v>1.9159999999999999</v>
       </c>
       <c r="J44" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K44" s="11">
         <v>3.9368400000000001</v>
@@ -3495,16 +3489,16 @@
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A45" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E45" s="11">
         <v>71.099999999999994</v>
@@ -3522,7 +3516,7 @@
         <v>3.1284000000000001</v>
       </c>
       <c r="J45" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K45" s="11">
         <v>3.6863000000000001</v>
@@ -3550,16 +3544,16 @@
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A46" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E46" s="12">
         <v>66.3</v>
@@ -3577,7 +3571,7 @@
         <v>2.5474600000000001</v>
       </c>
       <c r="J46" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K46" s="12">
         <v>3.7233999999999998</v>
@@ -3605,16 +3599,16 @@
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A47" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E47" s="12">
         <v>65.900000000000006</v>
@@ -3632,7 +3626,7 @@
         <v>1.7962</v>
       </c>
       <c r="J47" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K47" s="12">
         <v>3.9609999999999999</v>
@@ -3660,16 +3654,16 @@
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A48" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E48" s="12">
         <v>69.599999999999994</v>
@@ -3687,7 +3681,7 @@
         <v>2.0257999999999998</v>
       </c>
       <c r="J48" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K48" s="12">
         <v>3.887</v>
@@ -3715,16 +3709,16 @@
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A49" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E49" s="11">
         <v>73.599999999999994</v>
@@ -3742,7 +3736,7 @@
         <v>1.95285</v>
       </c>
       <c r="J49" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K49" s="11">
         <v>2.5710000000000002</v>
@@ -3770,16 +3764,16 @@
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A50" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E50" s="11">
         <v>64.400000000000006</v>
@@ -3797,7 +3791,7 @@
         <v>2.6345000000000001</v>
       </c>
       <c r="J50" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K50" s="11">
         <v>3.5470000000000002</v>
@@ -3825,16 +3819,16 @@
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A51" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E51" s="11">
         <v>46</v>
@@ -3852,7 +3846,7 @@
         <v>3.0129999999999999</v>
       </c>
       <c r="J51" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K51" s="11">
         <v>3.3290000000000002</v>
@@ -3877,7 +3871,7 @@
       <c r="Q51" s="17">
         <v>0.1233333333</v>
       </c>
-      <c r="R51" s="20"/>
+      <c r="R51" s="17"/>
       <c r="S51" s="17"/>
       <c r="T51" s="17"/>
       <c r="U51" s="17"/>
@@ -3887,16 +3881,16 @@
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A52" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E52" s="12">
         <v>49.5</v>
@@ -3914,7 +3908,7 @@
         <v>3.1241300000000001</v>
       </c>
       <c r="J52" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K52" s="12">
         <v>3.2215500000000001</v>
@@ -3942,16 +3936,16 @@
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A53" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E53" s="11">
         <v>70</v>
@@ -3969,7 +3963,7 @@
         <v>1.7764500000000001</v>
       </c>
       <c r="J53" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K53" s="11">
         <v>4.3869999999999996</v>
@@ -3997,16 +3991,16 @@
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A54" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E54" s="12">
         <v>36.6</v>
@@ -4024,7 +4018,7 @@
         <v>1.7669999999999999</v>
       </c>
       <c r="J54" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K54" s="12">
         <v>2.79</v>
@@ -4052,16 +4046,16 @@
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A55" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E55" s="12">
         <v>51.6</v>
@@ -4079,7 +4073,7 @@
         <v>2.27298</v>
       </c>
       <c r="J55" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K55" s="12">
         <v>3.0575000000000001</v>
@@ -4107,16 +4101,16 @@
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A56" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E56" s="15">
         <v>49.1</v>
@@ -4134,7 +4128,7 @@
         <v>2.4161999999999999</v>
       </c>
       <c r="J56" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K56" s="15">
         <v>5.1167999999999996</v>
@@ -4162,16 +4156,16 @@
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A57" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E57" s="11">
         <v>49.2</v>
@@ -4189,7 +4183,7 @@
         <v>1.9827999999999999</v>
       </c>
       <c r="J57" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K57" s="11">
         <v>2.7288999999999999</v>
@@ -4217,16 +4211,16 @@
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A58" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E58" s="11">
         <v>70.599999999999994</v>
@@ -4244,7 +4238,7 @@
         <v>2.7212499999999999</v>
       </c>
       <c r="J58" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K58" s="11">
         <v>4.7807000000000004</v>
@@ -4280,16 +4274,16 @@
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A59" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E59" s="12">
         <v>63.5</v>
@@ -4307,7 +4301,7 @@
         <v>1.863</v>
       </c>
       <c r="J59" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K59" s="12">
         <v>3.0373999999999999</v>
@@ -4335,16 +4329,16 @@
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A60" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E60" s="12">
         <v>67.099999999999994</v>
@@ -4362,7 +4356,7 @@
         <v>3.1240000000000001</v>
       </c>
       <c r="J60" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K60" s="12">
         <v>4.7484999999999999</v>
@@ -4390,16 +4384,16 @@
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A61" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E61" s="11">
         <v>67.599999999999994</v>
@@ -4417,7 +4411,7 @@
         <v>1.9018699999999999</v>
       </c>
       <c r="J61" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K61" s="11">
         <v>4.9688800000000004</v>
@@ -4445,16 +4439,16 @@
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A62" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E62" s="12">
         <v>65.3</v>
@@ -4472,7 +4466,7 @@
         <v>2.3765000000000001</v>
       </c>
       <c r="J62" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K62" s="12">
         <v>2.5247999999999999</v>
@@ -4500,16 +4494,16 @@
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A63" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E63" s="12">
         <v>68.5</v>
@@ -4527,7 +4521,7 @@
         <v>2.5518000000000001</v>
       </c>
       <c r="J63" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K63" s="12">
         <v>3.4788999999999999</v>
@@ -4555,16 +4549,16 @@
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A64" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E64" s="11">
         <v>73.400000000000006</v>
@@ -4582,7 +4576,7 @@
         <v>1.635</v>
       </c>
       <c r="J64" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K64" s="11">
         <v>3.7210000000000001</v>
@@ -4610,16 +4604,16 @@
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A65" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E65" s="4">
         <v>67.599999999999994</v>
@@ -4637,7 +4631,7 @@
         <v>2.5036</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K65" s="4">
         <v>2.3212999999999999</v>
@@ -4665,16 +4659,16 @@
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A66" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E66" s="11">
         <v>48.5</v>
@@ -4692,7 +4686,7 @@
         <v>2.12724</v>
       </c>
       <c r="J66" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K66" s="11">
         <v>4.0191999999999997</v>
@@ -4728,16 +4722,16 @@
     </row>
     <row r="67" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A67" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E67" s="11">
         <v>45.9</v>
@@ -4755,7 +4749,7 @@
         <v>2.11605</v>
       </c>
       <c r="J67" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K67" s="11">
         <v>2.65</v>
@@ -4783,16 +4777,16 @@
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A68" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E68" s="12">
         <v>47</v>
@@ -4810,7 +4804,7 @@
         <v>2.0916999999999999</v>
       </c>
       <c r="J68" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K68" s="12">
         <v>3.31</v>
@@ -4838,16 +4832,16 @@
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A69" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E69" s="12">
         <v>49.5</v>
@@ -4865,7 +4859,7 @@
         <v>3.1280999999999999</v>
       </c>
       <c r="J69" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K69" s="12">
         <v>4.92</v>
@@ -4893,16 +4887,16 @@
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A70" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E70" s="12">
         <v>45.8</v>
@@ -4920,7 +4914,7 @@
         <v>1.3939999999999999</v>
       </c>
       <c r="J70" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K70" s="12">
         <v>2.8250000000000002</v>
@@ -4948,16 +4942,16 @@
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A71" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E71" s="12">
         <v>49.2</v>
@@ -4975,7 +4969,7 @@
         <v>4.0117000000000003</v>
       </c>
       <c r="J71" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K71" s="12">
         <v>2.4489000000000001</v>
@@ -5003,16 +4997,16 @@
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A72" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D72" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E72" s="12">
         <v>51.9</v>
@@ -5030,7 +5024,7 @@
         <v>2.9929999999999999</v>
       </c>
       <c r="J72" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K72" s="12">
         <v>2.8918400000000002</v>
@@ -5058,16 +5052,16 @@
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A73" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E73" s="1">
         <v>45.5</v>
@@ -5085,7 +5079,7 @@
         <v>2.4567399999999999</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K73" s="1">
         <v>4.3175999999999997</v>
@@ -5113,16 +5107,16 @@
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A74" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E74" s="11">
         <v>74.2</v>
@@ -5140,7 +5134,7 @@
         <v>1.4196</v>
       </c>
       <c r="J74" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K74" s="11">
         <v>3.8727999999999998</v>
@@ -5176,16 +5170,16 @@
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A75" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D75" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E75" s="12">
         <v>71.2</v>
@@ -5203,7 +5197,7 @@
         <v>4.609</v>
       </c>
       <c r="J75" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K75" s="12">
         <v>3.1230799999999999</v>
@@ -5231,16 +5225,16 @@
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A76" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E76" s="12">
         <v>63.8</v>
@@ -5258,7 +5252,7 @@
         <v>2.3763000000000001</v>
       </c>
       <c r="J76" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K76" s="12">
         <v>6.3970000000000002</v>
@@ -5286,16 +5280,16 @@
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A77" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E77" s="12">
         <v>70.7</v>
@@ -5313,7 +5307,7 @@
         <v>2.3033600000000001</v>
       </c>
       <c r="J77" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K77" s="12">
         <v>4.7939999999999996</v>
@@ -5341,16 +5335,16 @@
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A78" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D78" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E78" s="12">
         <v>70.400000000000006</v>
@@ -5368,7 +5362,7 @@
         <v>2.1425999999999998</v>
       </c>
       <c r="J78" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K78" s="12">
         <v>2.9790000000000001</v>
@@ -5396,16 +5390,16 @@
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A79" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D79" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E79" s="12">
         <v>67.8</v>
@@ -5423,7 +5417,7 @@
         <v>1.71004</v>
       </c>
       <c r="J79" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K79" s="12">
         <v>4.1809200000000004</v>
@@ -5451,16 +5445,16 @@
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A80" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D80" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E80" s="12">
         <v>68.099999999999994</v>
@@ -5478,7 +5472,7 @@
         <v>3.1859600000000001</v>
       </c>
       <c r="J80" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K80" s="12">
         <v>5.5270000000000001</v>
@@ -5506,16 +5500,16 @@
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A81" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E81" s="1">
         <v>70.900000000000006</v>
@@ -5533,7 +5527,7 @@
         <v>1.9716</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K81" s="1">
         <v>3.1267999999999998</v>
@@ -5561,16 +5555,16 @@
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A82" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D82" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E82" s="12">
         <v>49.6</v>
@@ -5588,7 +5582,7 @@
         <v>2.718</v>
       </c>
       <c r="J82" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K82" s="12">
         <v>3.6110000000000002</v>
@@ -5625,16 +5619,16 @@
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A83" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E83" s="11">
         <v>49.5</v>
@@ -5652,7 +5646,7 @@
         <v>2.1617000000000002</v>
       </c>
       <c r="J83" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K83" s="11">
         <v>5.0259999999999998</v>
@@ -5680,16 +5674,16 @@
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A84" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D84" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E84" s="12">
         <v>49.4</v>
@@ -5707,7 +5701,7 @@
         <v>1.99932</v>
       </c>
       <c r="J84" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K84" s="12">
         <v>3.5070000000000001</v>
@@ -5735,16 +5729,16 @@
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A85" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D85" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E85" s="12">
         <v>43.7</v>
@@ -5762,7 +5756,7 @@
         <v>2.0352999999999999</v>
       </c>
       <c r="J85" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K85" s="14">
         <v>4.5407999999999999</v>
@@ -5790,16 +5784,16 @@
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A86" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E86" s="11">
         <v>45.9</v>
@@ -5810,14 +5804,12 @@
       <c r="G86" s="11">
         <v>2.105</v>
       </c>
-      <c r="H86" s="11" t="s">
-        <v>14</v>
-      </c>
+      <c r="H86" s="11"/>
       <c r="I86" s="11">
         <v>1.615</v>
       </c>
       <c r="J86" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K86" s="11">
         <v>4.55</v>
@@ -5845,16 +5837,16 @@
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A87" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D87" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E87" s="12">
         <v>47.3</v>
@@ -5872,7 +5864,7 @@
         <v>1.859</v>
       </c>
       <c r="J87" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K87" s="12">
         <v>3.2374999999999998</v>
@@ -5900,16 +5892,16 @@
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A88" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E88" s="11">
         <v>46.4</v>
@@ -5927,7 +5919,7 @@
         <v>2.4551400000000001</v>
       </c>
       <c r="J88" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K88" s="11">
         <v>3.3570000000000002</v>
@@ -5955,16 +5947,16 @@
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A89" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E89" s="1">
         <v>152</v>
@@ -5982,7 +5974,7 @@
         <v>0.61060000000000003</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K89" s="1">
         <v>0.75229999999999997</v>
@@ -6010,16 +6002,16 @@
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A90" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E90" s="1">
         <v>45.8</v>
@@ -6037,7 +6029,7 @@
         <v>1.9335</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K90" s="1">
         <v>3.919</v>

</xml_diff>

<commit_message>
Creating a new dataset for transpiration rates
</commit_message>
<xml_diff>
--- a/Harvest Data.xlsx
+++ b/Harvest Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/demoriegalarza/Desktop/DFD+DAG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2362D75-4550-704A-99B5-DD52620A11C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195582A7-3F9B-B541-90D4-10E066F3FD36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4400" yWindow="500" windowWidth="21200" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="205">
   <si>
     <t>NM31</t>
   </si>
@@ -288,9 +288,6 @@
   </si>
   <si>
     <t>DFD_042</t>
-  </si>
-  <si>
-    <t>50.4*</t>
   </si>
   <si>
     <t>NM35</t>
@@ -1014,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819B6F9D-1188-934E-9CF0-4A8F8C7DD01E}">
   <dimension ref="A1:Z90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1031,55 +1028,55 @@
   <sheetData>
     <row r="1" spans="1:24" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>184</v>
-      </c>
       <c r="J1" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="P1" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.15">
@@ -1090,10 +1087,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E2" s="1">
         <v>60.6</v>
@@ -1111,7 +1108,7 @@
         <v>1.3979999999999999</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K2" s="1">
         <v>4.29</v>
@@ -1151,10 +1148,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E3" s="1">
         <v>70</v>
@@ -1172,7 +1169,7 @@
         <v>2.0470000000000002</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K3" s="1">
         <v>3.8035199999999998</v>
@@ -1206,10 +1203,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E4" s="2">
         <v>74.099999999999994</v>
@@ -1227,7 +1224,7 @@
         <v>1.133</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K4" s="2">
         <v>1.958</v>
@@ -1261,10 +1258,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E5" s="2">
         <v>81.599999999999994</v>
@@ -1282,7 +1279,7 @@
         <v>1.212</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K5" s="2">
         <v>2.0289999999999999</v>
@@ -1316,10 +1313,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E6" s="1">
         <v>61.2</v>
@@ -1337,7 +1334,7 @@
         <v>2.2440000000000002</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K6" s="1">
         <v>3.82185</v>
@@ -1371,10 +1368,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E7" s="2">
         <v>65.8</v>
@@ -1392,7 +1389,7 @@
         <v>1.611</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K7" s="2">
         <v>2.0356000000000001</v>
@@ -1426,10 +1423,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E8" s="1">
         <v>70.099999999999994</v>
@@ -1447,7 +1444,7 @@
         <v>1.4984</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K8" s="1">
         <v>3.448</v>
@@ -1481,10 +1478,10 @@
         <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E9" s="1">
         <v>50.1</v>
@@ -1502,7 +1499,7 @@
         <v>3.0030000000000001</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K9" s="1">
         <v>3.4780000000000002</v>
@@ -1543,10 +1540,10 @@
         <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E10" s="1">
         <v>52.5</v>
@@ -1564,7 +1561,7 @@
         <v>1.2791600000000001</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K10" s="1">
         <v>0.78600000000000003</v>
@@ -1598,10 +1595,10 @@
         <v>16</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E11" s="2">
         <v>48.3</v>
@@ -1619,7 +1616,7 @@
         <v>2.1102400000000001</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K11" s="2">
         <v>6.1619999999999999</v>
@@ -1653,10 +1650,10 @@
         <v>17</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E12" s="4">
         <v>50</v>
@@ -1674,7 +1671,7 @@
         <v>2.0700099999999999</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K12" s="4">
         <v>3.72</v>
@@ -1708,10 +1705,10 @@
         <v>18</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E13" s="1">
         <v>51.7</v>
@@ -1729,7 +1726,7 @@
         <v>1.9006000000000001</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K13" s="1">
         <v>2.0390000000000001</v>
@@ -1763,10 +1760,10 @@
         <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E14" s="2">
         <v>48.7</v>
@@ -1784,7 +1781,7 @@
         <v>2.7336999999999998</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K14" s="2">
         <v>3.875</v>
@@ -1818,10 +1815,10 @@
         <v>20</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E15" s="2">
         <v>48.6</v>
@@ -1839,7 +1836,7 @@
         <v>1.88849</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K15" s="2">
         <v>3.6259999999999999</v>
@@ -1873,10 +1870,10 @@
         <v>28</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E16" s="1">
         <v>69.900000000000006</v>
@@ -1894,7 +1891,7 @@
         <v>2.5703</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K16" s="1">
         <v>1.8180000000000001</v>
@@ -1935,10 +1932,10 @@
         <v>29</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E17" s="1">
         <v>69.400000000000006</v>
@@ -1956,7 +1953,7 @@
         <v>2.2650000000000001</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K17" s="1">
         <v>3.0270000000000001</v>
@@ -1990,10 +1987,10 @@
         <v>30</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E18" s="2">
         <v>80.5</v>
@@ -2011,7 +2008,7 @@
         <v>1.2509999999999999</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K18" s="2">
         <v>3.0179999999999998</v>
@@ -2045,10 +2042,10 @@
         <v>31</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E19" s="4">
         <v>67.7</v>
@@ -2066,7 +2063,7 @@
         <v>1.7380899999999999</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K19" s="4">
         <v>0.52300000000000002</v>
@@ -2098,10 +2095,10 @@
         <v>32</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E20" s="2">
         <v>61</v>
@@ -2119,7 +2116,7 @@
         <v>3.0325600000000001</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K20" s="2">
         <v>4.766</v>
@@ -2151,10 +2148,10 @@
         <v>33</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E21" s="1">
         <v>67.3</v>
@@ -2172,7 +2169,7 @@
         <v>3.3971</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K21" s="1">
         <v>4.49</v>
@@ -2206,10 +2203,10 @@
         <v>34</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E22" s="1">
         <v>71.8</v>
@@ -2225,7 +2222,7 @@
         <v>2.5780099999999999</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K22" s="1">
         <v>2.238</v>
@@ -2259,10 +2256,10 @@
         <v>42</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E23" s="1">
         <v>49.5</v>
@@ -2280,7 +2277,7 @@
         <v>2.7604000000000002</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K23" s="1">
         <v>3.4950000000000001</v>
@@ -2321,10 +2318,10 @@
         <v>43</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E24" s="1">
         <v>44.9</v>
@@ -2342,7 +2339,7 @@
         <v>2.206</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K24" s="1">
         <v>4.1120000000000001</v>
@@ -2376,10 +2373,10 @@
         <v>44</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E25" s="1">
         <v>46.7</v>
@@ -2397,7 +2394,7 @@
         <v>2.14</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K25" s="1">
         <v>3.1970000000000001</v>
@@ -2431,10 +2428,10 @@
         <v>45</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E26" s="1">
         <v>73.099999999999994</v>
@@ -2452,7 +2449,7 @@
         <v>1.4770000000000001</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K26" s="1">
         <v>1.4357</v>
@@ -2486,10 +2483,10 @@
         <v>46</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E27" s="2">
         <v>47.5</v>
@@ -2507,7 +2504,7 @@
         <v>2.8519999999999999</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K27" s="2">
         <v>3.6659999999999999</v>
@@ -2541,10 +2538,10 @@
         <v>47</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E28" s="2">
         <v>49.3</v>
@@ -2562,7 +2559,7 @@
         <v>1.3718600000000001</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K28" s="2">
         <v>2.8759999999999999</v>
@@ -2596,10 +2593,10 @@
         <v>48</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E29" s="2">
         <v>51.2</v>
@@ -2617,7 +2614,7 @@
         <v>2.6284999999999998</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K29" s="2">
         <v>4.93</v>
@@ -2651,10 +2648,10 @@
         <v>56</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E30" s="5">
         <v>67.599999999999994</v>
@@ -2672,7 +2669,7 @@
         <v>3.1321300000000001</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K30" s="5">
         <v>2.5648</v>
@@ -2713,10 +2710,10 @@
         <v>57</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E31" s="6">
         <v>64.599999999999994</v>
@@ -2734,7 +2731,7 @@
         <v>1.7172000000000001</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K31" s="10">
         <v>5.2245999999999997</v>
@@ -2768,10 +2765,10 @@
         <v>58</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E32" s="7">
         <v>67.400000000000006</v>
@@ -2789,7 +2786,7 @@
         <v>2.8140000000000001</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K32" s="7">
         <v>7.1459999999999999</v>
@@ -2823,10 +2820,10 @@
         <v>59</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E33" s="6">
         <v>69</v>
@@ -2844,7 +2841,7 @@
         <v>1.9293</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K33" s="10">
         <v>4.0349000000000004</v>
@@ -2878,10 +2875,10 @@
         <v>60</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E34" s="5">
         <v>69</v>
@@ -2899,7 +2896,7 @@
         <v>1.583</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K34" s="5">
         <v>5.3268000000000004</v>
@@ -2933,10 +2930,10 @@
         <v>61</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E35" s="5">
         <v>64.2</v>
@@ -2954,7 +2951,7 @@
         <v>2.2183099999999998</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K35" s="5">
         <v>2.3675000000000002</v>
@@ -2988,10 +2985,10 @@
         <v>62</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E36" s="7">
         <v>71.2</v>
@@ -3009,7 +3006,7 @@
         <v>1.26955</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K36" s="7">
         <v>2.819</v>
@@ -3043,10 +3040,10 @@
         <v>70</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E37" s="11">
         <v>46.5</v>
@@ -3064,7 +3061,7 @@
         <v>2.2846299999999999</v>
       </c>
       <c r="J37" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K37" s="11">
         <v>8.01</v>
@@ -3103,10 +3100,10 @@
         <v>71</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E38" s="12">
         <v>46.7</v>
@@ -3124,7 +3121,7 @@
         <v>1.5205299999999999</v>
       </c>
       <c r="J38" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K38" s="14">
         <v>5.5625999999999998</v>
@@ -3158,10 +3155,10 @@
         <v>72</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E39" s="12">
         <v>46</v>
@@ -3179,7 +3176,7 @@
         <v>1.7919</v>
       </c>
       <c r="J39" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K39" s="12">
         <v>2.9994999999999998</v>
@@ -3213,10 +3210,10 @@
         <v>73</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E40" s="11">
         <v>129.6</v>
@@ -3234,7 +3231,7 @@
         <v>1.38964</v>
       </c>
       <c r="J40" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K40" s="13">
         <v>0.41494999999999999</v>
@@ -3268,13 +3265,13 @@
         <v>74</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="E41" s="12" t="s">
-        <v>84</v>
+        <v>201</v>
+      </c>
+      <c r="E41" s="12">
+        <v>50.4</v>
       </c>
       <c r="F41" s="12">
         <v>1.9</v>
@@ -3289,7 +3286,7 @@
         <v>1.1151</v>
       </c>
       <c r="J41" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K41" s="12">
         <v>2.2669999999999999</v>
@@ -3323,10 +3320,10 @@
         <v>75</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E42" s="11">
         <v>48.4</v>
@@ -3344,7 +3341,7 @@
         <v>2.4632999999999998</v>
       </c>
       <c r="J42" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K42" s="11">
         <v>4.4850000000000003</v>
@@ -3378,10 +3375,10 @@
         <v>76</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E43" s="11">
         <v>56.6</v>
@@ -3399,7 +3396,7 @@
         <v>2.3729800000000001</v>
       </c>
       <c r="J43" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K43" s="11">
         <v>2.14</v>
@@ -3427,16 +3424,16 @@
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A44" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E44" s="11">
         <v>67.5</v>
@@ -3454,7 +3451,7 @@
         <v>1.9159999999999999</v>
       </c>
       <c r="J44" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K44" s="11">
         <v>3.9368400000000001</v>
@@ -3489,16 +3486,16 @@
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A45" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E45" s="11">
         <v>71.099999999999994</v>
@@ -3516,7 +3513,7 @@
         <v>3.1284000000000001</v>
       </c>
       <c r="J45" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K45" s="11">
         <v>3.6863000000000001</v>
@@ -3544,16 +3541,16 @@
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A46" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E46" s="12">
         <v>66.3</v>
@@ -3571,7 +3568,7 @@
         <v>2.5474600000000001</v>
       </c>
       <c r="J46" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K46" s="12">
         <v>3.7233999999999998</v>
@@ -3599,16 +3596,16 @@
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A47" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E47" s="12">
         <v>65.900000000000006</v>
@@ -3626,7 +3623,7 @@
         <v>1.7962</v>
       </c>
       <c r="J47" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K47" s="12">
         <v>3.9609999999999999</v>
@@ -3654,16 +3651,16 @@
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A48" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E48" s="12">
         <v>69.599999999999994</v>
@@ -3681,7 +3678,7 @@
         <v>2.0257999999999998</v>
       </c>
       <c r="J48" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K48" s="12">
         <v>3.887</v>
@@ -3709,16 +3706,16 @@
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A49" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E49" s="11">
         <v>73.599999999999994</v>
@@ -3736,7 +3733,7 @@
         <v>1.95285</v>
       </c>
       <c r="J49" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K49" s="11">
         <v>2.5710000000000002</v>
@@ -3764,16 +3761,16 @@
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A50" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E50" s="11">
         <v>64.400000000000006</v>
@@ -3791,7 +3788,7 @@
         <v>2.6345000000000001</v>
       </c>
       <c r="J50" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K50" s="11">
         <v>3.5470000000000002</v>
@@ -3819,16 +3816,16 @@
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A51" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E51" s="11">
         <v>46</v>
@@ -3846,7 +3843,7 @@
         <v>3.0129999999999999</v>
       </c>
       <c r="J51" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K51" s="11">
         <v>3.3290000000000002</v>
@@ -3881,16 +3878,16 @@
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A52" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E52" s="12">
         <v>49.5</v>
@@ -3908,7 +3905,7 @@
         <v>3.1241300000000001</v>
       </c>
       <c r="J52" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K52" s="12">
         <v>3.2215500000000001</v>
@@ -3936,16 +3933,16 @@
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A53" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E53" s="11">
         <v>70</v>
@@ -3963,7 +3960,7 @@
         <v>1.7764500000000001</v>
       </c>
       <c r="J53" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K53" s="11">
         <v>4.3869999999999996</v>
@@ -3991,16 +3988,16 @@
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A54" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E54" s="12">
         <v>36.6</v>
@@ -4018,7 +4015,7 @@
         <v>1.7669999999999999</v>
       </c>
       <c r="J54" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K54" s="12">
         <v>2.79</v>
@@ -4046,16 +4043,16 @@
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A55" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E55" s="12">
         <v>51.6</v>
@@ -4073,7 +4070,7 @@
         <v>2.27298</v>
       </c>
       <c r="J55" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K55" s="12">
         <v>3.0575000000000001</v>
@@ -4101,16 +4098,16 @@
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A56" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E56" s="15">
         <v>49.1</v>
@@ -4128,7 +4125,7 @@
         <v>2.4161999999999999</v>
       </c>
       <c r="J56" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K56" s="15">
         <v>5.1167999999999996</v>
@@ -4156,16 +4153,16 @@
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A57" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E57" s="11">
         <v>49.2</v>
@@ -4183,7 +4180,7 @@
         <v>1.9827999999999999</v>
       </c>
       <c r="J57" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K57" s="11">
         <v>2.7288999999999999</v>
@@ -4211,16 +4208,16 @@
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A58" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E58" s="11">
         <v>70.599999999999994</v>
@@ -4238,7 +4235,7 @@
         <v>2.7212499999999999</v>
       </c>
       <c r="J58" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K58" s="11">
         <v>4.7807000000000004</v>
@@ -4274,16 +4271,16 @@
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A59" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E59" s="12">
         <v>63.5</v>
@@ -4301,7 +4298,7 @@
         <v>1.863</v>
       </c>
       <c r="J59" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K59" s="12">
         <v>3.0373999999999999</v>
@@ -4329,16 +4326,16 @@
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A60" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E60" s="12">
         <v>67.099999999999994</v>
@@ -4356,7 +4353,7 @@
         <v>3.1240000000000001</v>
       </c>
       <c r="J60" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K60" s="12">
         <v>4.7484999999999999</v>
@@ -4384,16 +4381,16 @@
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A61" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E61" s="11">
         <v>67.599999999999994</v>
@@ -4411,7 +4408,7 @@
         <v>1.9018699999999999</v>
       </c>
       <c r="J61" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K61" s="11">
         <v>4.9688800000000004</v>
@@ -4439,16 +4436,16 @@
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A62" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E62" s="12">
         <v>65.3</v>
@@ -4466,7 +4463,7 @@
         <v>2.3765000000000001</v>
       </c>
       <c r="J62" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K62" s="12">
         <v>2.5247999999999999</v>
@@ -4494,16 +4491,16 @@
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A63" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E63" s="12">
         <v>68.5</v>
@@ -4521,7 +4518,7 @@
         <v>2.5518000000000001</v>
       </c>
       <c r="J63" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K63" s="12">
         <v>3.4788999999999999</v>
@@ -4549,16 +4546,16 @@
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A64" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E64" s="11">
         <v>73.400000000000006</v>
@@ -4576,7 +4573,7 @@
         <v>1.635</v>
       </c>
       <c r="J64" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K64" s="11">
         <v>3.7210000000000001</v>
@@ -4604,16 +4601,16 @@
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A65" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E65" s="4">
         <v>67.599999999999994</v>
@@ -4631,7 +4628,7 @@
         <v>2.5036</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K65" s="4">
         <v>2.3212999999999999</v>
@@ -4659,16 +4656,16 @@
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A66" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E66" s="11">
         <v>48.5</v>
@@ -4686,7 +4683,7 @@
         <v>2.12724</v>
       </c>
       <c r="J66" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K66" s="11">
         <v>4.0191999999999997</v>
@@ -4722,16 +4719,16 @@
     </row>
     <row r="67" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A67" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E67" s="11">
         <v>45.9</v>
@@ -4749,7 +4746,7 @@
         <v>2.11605</v>
       </c>
       <c r="J67" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K67" s="11">
         <v>2.65</v>
@@ -4777,16 +4774,16 @@
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A68" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E68" s="12">
         <v>47</v>
@@ -4804,7 +4801,7 @@
         <v>2.0916999999999999</v>
       </c>
       <c r="J68" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K68" s="12">
         <v>3.31</v>
@@ -4832,16 +4829,16 @@
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A69" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E69" s="12">
         <v>49.5</v>
@@ -4859,7 +4856,7 @@
         <v>3.1280999999999999</v>
       </c>
       <c r="J69" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K69" s="12">
         <v>4.92</v>
@@ -4887,16 +4884,16 @@
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A70" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E70" s="12">
         <v>45.8</v>
@@ -4914,7 +4911,7 @@
         <v>1.3939999999999999</v>
       </c>
       <c r="J70" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K70" s="12">
         <v>2.8250000000000002</v>
@@ -4942,16 +4939,16 @@
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A71" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E71" s="12">
         <v>49.2</v>
@@ -4969,7 +4966,7 @@
         <v>4.0117000000000003</v>
       </c>
       <c r="J71" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K71" s="12">
         <v>2.4489000000000001</v>
@@ -4997,16 +4994,16 @@
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A72" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D72" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E72" s="12">
         <v>51.9</v>
@@ -5024,7 +5021,7 @@
         <v>2.9929999999999999</v>
       </c>
       <c r="J72" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K72" s="12">
         <v>2.8918400000000002</v>
@@ -5052,16 +5049,16 @@
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A73" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E73" s="1">
         <v>45.5</v>
@@ -5079,7 +5076,7 @@
         <v>2.4567399999999999</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K73" s="1">
         <v>4.3175999999999997</v>
@@ -5107,16 +5104,16 @@
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A74" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E74" s="11">
         <v>74.2</v>
@@ -5134,7 +5131,7 @@
         <v>1.4196</v>
       </c>
       <c r="J74" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K74" s="11">
         <v>3.8727999999999998</v>
@@ -5170,16 +5167,16 @@
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A75" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D75" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E75" s="12">
         <v>71.2</v>
@@ -5197,7 +5194,7 @@
         <v>4.609</v>
       </c>
       <c r="J75" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K75" s="12">
         <v>3.1230799999999999</v>
@@ -5225,16 +5222,16 @@
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A76" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E76" s="12">
         <v>63.8</v>
@@ -5252,7 +5249,7 @@
         <v>2.3763000000000001</v>
       </c>
       <c r="J76" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K76" s="12">
         <v>6.3970000000000002</v>
@@ -5280,16 +5277,16 @@
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A77" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E77" s="12">
         <v>70.7</v>
@@ -5307,7 +5304,7 @@
         <v>2.3033600000000001</v>
       </c>
       <c r="J77" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K77" s="12">
         <v>4.7939999999999996</v>
@@ -5335,16 +5332,16 @@
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A78" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D78" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E78" s="12">
         <v>70.400000000000006</v>
@@ -5362,7 +5359,7 @@
         <v>2.1425999999999998</v>
       </c>
       <c r="J78" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K78" s="12">
         <v>2.9790000000000001</v>
@@ -5390,16 +5387,16 @@
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A79" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D79" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E79" s="12">
         <v>67.8</v>
@@ -5417,7 +5414,7 @@
         <v>1.71004</v>
       </c>
       <c r="J79" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K79" s="12">
         <v>4.1809200000000004</v>
@@ -5445,16 +5442,16 @@
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A80" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D80" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E80" s="12">
         <v>68.099999999999994</v>
@@ -5472,7 +5469,7 @@
         <v>3.1859600000000001</v>
       </c>
       <c r="J80" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K80" s="12">
         <v>5.5270000000000001</v>
@@ -5500,16 +5497,16 @@
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A81" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E81" s="1">
         <v>70.900000000000006</v>
@@ -5527,7 +5524,7 @@
         <v>1.9716</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K81" s="1">
         <v>3.1267999999999998</v>
@@ -5555,16 +5552,16 @@
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A82" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D82" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E82" s="12">
         <v>49.6</v>
@@ -5582,7 +5579,7 @@
         <v>2.718</v>
       </c>
       <c r="J82" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K82" s="12">
         <v>3.6110000000000002</v>
@@ -5619,16 +5616,16 @@
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A83" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E83" s="11">
         <v>49.5</v>
@@ -5646,7 +5643,7 @@
         <v>2.1617000000000002</v>
       </c>
       <c r="J83" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K83" s="11">
         <v>5.0259999999999998</v>
@@ -5674,16 +5671,16 @@
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A84" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D84" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E84" s="12">
         <v>49.4</v>
@@ -5701,7 +5698,7 @@
         <v>1.99932</v>
       </c>
       <c r="J84" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K84" s="12">
         <v>3.5070000000000001</v>
@@ -5729,16 +5726,16 @@
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A85" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D85" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E85" s="12">
         <v>43.7</v>
@@ -5756,7 +5753,7 @@
         <v>2.0352999999999999</v>
       </c>
       <c r="J85" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K85" s="14">
         <v>4.5407999999999999</v>
@@ -5784,16 +5781,16 @@
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A86" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E86" s="11">
         <v>45.9</v>
@@ -5809,7 +5806,7 @@
         <v>1.615</v>
       </c>
       <c r="J86" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K86" s="11">
         <v>4.55</v>
@@ -5837,16 +5834,16 @@
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A87" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D87" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E87" s="12">
         <v>47.3</v>
@@ -5864,7 +5861,7 @@
         <v>1.859</v>
       </c>
       <c r="J87" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K87" s="12">
         <v>3.2374999999999998</v>
@@ -5892,16 +5889,16 @@
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A88" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E88" s="11">
         <v>46.4</v>
@@ -5919,7 +5916,7 @@
         <v>2.4551400000000001</v>
       </c>
       <c r="J88" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K88" s="11">
         <v>3.3570000000000002</v>
@@ -5947,16 +5944,16 @@
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A89" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E89" s="1">
         <v>152</v>
@@ -5974,7 +5971,7 @@
         <v>0.61060000000000003</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K89" s="1">
         <v>0.75229999999999997</v>
@@ -6002,16 +5999,16 @@
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A90" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E90" s="1">
         <v>45.8</v>
@@ -6029,7 +6026,7 @@
         <v>1.9335</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K90" s="1">
         <v>3.919</v>

</xml_diff>